<commit_message>
added function to test all models
</commit_message>
<xml_diff>
--- a/Bioc/Dane.xlsx
+++ b/Bioc/Dane.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,7 +461,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>modelCNN.model</t>
+          <t>modelSVM.pkl</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -469,11 +469,9 @@
           <t>audio files/</t>
         </is>
       </c>
-      <c r="D2" t="n">
-        <v>0.4256819188594818</v>
-      </c>
+      <c r="D2" t="inlineStr"/>
       <c r="E2" t="n">
-        <v>0.894859790802002</v>
+        <v>0.9252336448598131</v>
       </c>
     </row>
     <row r="3">
@@ -482,7 +480,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>modelRNN.model</t>
+          <t>modelRandomForest.pkl</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -490,11 +488,9 @@
           <t>audio files/</t>
         </is>
       </c>
-      <c r="D3" t="n">
-        <v>0.1860886365175247</v>
-      </c>
+      <c r="D3" t="inlineStr"/>
       <c r="E3" t="n">
-        <v>0.9439252614974976</v>
+        <v>0.9485981308411215</v>
       </c>
     </row>
     <row r="4">
@@ -503,7 +499,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>modelMLP.model</t>
+          <t>modelCNN.model</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -512,10 +508,10 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>0.1019595563411713</v>
+        <v>0.4256819188594818</v>
       </c>
       <c r="E4" t="n">
-        <v>0.9742990732192993</v>
+        <v>0.894859790802002</v>
       </c>
     </row>
     <row r="5">
@@ -524,19 +520,19 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>modelCNN.model</t>
+          <t>modelRNN.model</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>files/</t>
+          <t>audio files/</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>3.569734334945679</v>
+        <v>0.1860886365175247</v>
       </c>
       <c r="E5" t="n">
-        <v>0.6206896305084229</v>
+        <v>0.9439252614974976</v>
       </c>
     </row>
     <row r="6">
@@ -545,19 +541,19 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>modelRNN.model</t>
+          <t>modelMLP.model</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>files/</t>
+          <t>audio files/</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>3.974804401397705</v>
+        <v>0.1019595563411713</v>
       </c>
       <c r="E6" t="n">
-        <v>0.1724137961864471</v>
+        <v>0.9742990732192993</v>
       </c>
     </row>
     <row r="7">
@@ -566,19 +562,99 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
+          <t>modelSVM.pkl</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>files/</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="n">
+        <v>0.1212121212121212</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>modelRandomForest.pkl</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>files/</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="n">
+        <v>0.5454545454545454</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>modelCNN.model</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>files/</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>3.656139612197876</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.6363636255264282</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>modelRNN.model</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>files/</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>3.805042266845703</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.1818181872367859</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
           <t>modelMLP.model</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="C11" t="inlineStr">
         <is>
           <t>files/</t>
         </is>
       </c>
-      <c r="D7" t="n">
-        <v>3.603017568588257</v>
-      </c>
-      <c r="E7" t="n">
-        <v>0.5862069129943848</v>
+      <c r="D11" t="n">
+        <v>3.09204888343811</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.6060606241226196</v>
       </c>
     </row>
   </sheetData>

</xml_diff>